<commit_message>
Futureyou calendar update - reject retainer shortlist, accept retainer completion
</commit_message>
<xml_diff>
--- a/H2coco/TradeFinance.xlsx
+++ b/H2coco/TradeFinance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Github/XeroAPI/H2coco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EF965E-5B3E-0042-BB55-05B7A47ED8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA43461-B675-874F-9561-9C5CFC325EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="-23760" windowWidth="28040" windowHeight="17440" xr2:uid="{FFDF8704-F7A6-5241-858B-D62B61F118F7}"/>
+    <workbookView xWindow="17580" yWindow="-24700" windowWidth="28040" windowHeight="17440" xr2:uid="{FFDF8704-F7A6-5241-858B-D62B61F118F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E04BC2-FCC1-F344-980C-32A6AB851348}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,27 +464,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>4099</v>
+        <v>4242</v>
       </c>
       <c r="B2" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C2" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D2" s="4">
-        <v>14586</v>
+        <v>29172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>4102</v>
+        <v>4244</v>
       </c>
       <c r="B3" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C3" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D3" s="4">
         <v>14586</v>
@@ -492,13 +492,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>4128</v>
+        <v>4256</v>
       </c>
       <c r="B4" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C4" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D4" s="4">
         <v>14586</v>
@@ -506,55 +506,55 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4243</v>
+        <v>4262</v>
       </c>
       <c r="B5" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C5" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D5" s="4">
-        <v>14586</v>
+        <v>14580.9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>4257</v>
+        <v>4263</v>
       </c>
       <c r="B6" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C6" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D6" s="4">
-        <v>14586</v>
+        <v>29172</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4283</v>
+        <v>4264</v>
       </c>
       <c r="B7" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C7" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D7" s="4">
-        <v>29172</v>
+        <v>14586</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>4297</v>
+        <v>4298</v>
       </c>
       <c r="B8" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C8" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D8" s="4">
         <v>14586</v>
@@ -562,13 +562,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>4318</v>
+        <v>4420</v>
       </c>
       <c r="B9" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C9" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D9" s="4">
         <v>14586</v>
@@ -576,13 +576,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>4319</v>
+        <v>4440</v>
       </c>
       <c r="B10" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C10" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D10" s="4">
         <v>14586</v>
@@ -590,167 +590,167 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>4369</v>
+        <v>4461</v>
       </c>
       <c r="B11" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C11" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D11" s="4">
-        <v>29172</v>
+        <v>14586</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>4372</v>
+        <v>4516</v>
       </c>
       <c r="B12" s="3">
-        <v>45939</v>
+        <v>45967</v>
       </c>
       <c r="C12" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65051000000000003</v>
       </c>
       <c r="D12" s="4">
-        <v>14586</v>
+        <v>14244.3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>4379</v>
+        <v>4766</v>
       </c>
       <c r="B13" s="3">
-        <v>45939</v>
+        <v>45974</v>
       </c>
       <c r="C13" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D13" s="4">
-        <v>14586</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>4384</v>
+        <v>4767</v>
       </c>
       <c r="B14" s="3">
-        <v>45939</v>
+        <v>45974</v>
       </c>
       <c r="C14" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D14" s="4">
-        <v>14586</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>4411</v>
+        <v>4768</v>
       </c>
       <c r="B15" s="3">
-        <v>45939</v>
+        <v>45974</v>
       </c>
       <c r="C15" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D15" s="4">
-        <v>14586</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>4421</v>
+        <v>4769</v>
       </c>
       <c r="B16" s="3">
-        <v>45939</v>
+        <v>45974</v>
       </c>
       <c r="C16" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D16" s="4">
-        <v>14586</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>4457</v>
+        <v>4470</v>
       </c>
       <c r="B17" s="3">
-        <v>45939</v>
+        <v>45974</v>
       </c>
       <c r="C17" s="2">
-        <v>0.65805000000000002</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D17" s="4">
-        <v>14586</v>
+        <v>8861.4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>4466</v>
+        <v>4540</v>
       </c>
       <c r="B18" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C18" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D18" s="4">
-        <v>3801.6</v>
+        <v>8870.4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>4561</v>
+        <v>4572</v>
       </c>
       <c r="B19" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C19" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D19" s="4">
-        <v>3538.08</v>
+        <v>8870.4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>4566</v>
+        <v>4574</v>
       </c>
       <c r="B20" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C20" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D20" s="4">
-        <v>3316.95</v>
+        <v>8870.4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>4569</v>
+        <v>4576</v>
       </c>
       <c r="B21" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C21" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65532999999999997</v>
       </c>
       <c r="D21" s="4">
-        <v>3801.6</v>
+        <v>8870.4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>4571</v>
+        <v>4396</v>
       </c>
       <c r="B22" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C22" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D22" s="4">
         <v>3801.6</v>
@@ -758,55 +758,55 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>4573</v>
+        <v>4564</v>
       </c>
       <c r="B23" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C23" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D23" s="4">
-        <v>3801.6</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>4630</v>
+        <v>4692</v>
       </c>
       <c r="B24" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C24" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D24" s="4">
-        <v>3979.95</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>4632</v>
+        <v>4700</v>
       </c>
       <c r="B25" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C25" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D25" s="4">
-        <v>3888.15</v>
+        <v>4160.7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>4633</v>
+        <v>4721</v>
       </c>
       <c r="B26" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C26" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D26" s="4">
         <v>4158</v>
@@ -814,240 +814,632 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>4634</v>
+        <v>4725</v>
       </c>
       <c r="B27" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C27" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D27" s="4">
-        <v>4114.95</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>4635</v>
+        <v>4749</v>
       </c>
       <c r="B28" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C28" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D28" s="4">
-        <v>3888.15</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>4636</v>
+        <v>4178</v>
       </c>
       <c r="B29" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C29" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D29" s="4">
-        <v>4158</v>
+        <v>9257.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>4231</v>
+        <v>4292</v>
       </c>
       <c r="B30" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C30" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D30" s="4">
-        <v>8357.4</v>
+        <v>8825.4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>4355</v>
+        <v>4441</v>
       </c>
       <c r="B31" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C31" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D31" s="4">
-        <v>8870.4</v>
+        <v>9751.32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>4389</v>
+        <v>4442</v>
       </c>
       <c r="B32" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C32" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D32" s="4">
-        <v>9487.7999999999993</v>
+        <v>9072.35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>4422</v>
+        <v>4443</v>
       </c>
       <c r="B33" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C33" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D33" s="4">
-        <v>9830.0400000000009</v>
+        <v>9286.5499999999993</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>4423</v>
+        <v>4462</v>
       </c>
       <c r="B34" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C34" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D34" s="4">
-        <v>8871.1</v>
+        <v>9286.5499999999993</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>4426</v>
+        <v>4495</v>
       </c>
       <c r="B35" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C35" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D35" s="4">
-        <v>9601.5499999999993</v>
+        <v>9526.44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>4427</v>
+        <v>4496</v>
       </c>
       <c r="B36" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C36" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D36" s="4">
-        <v>9841.44</v>
+        <v>9830.0400000000009</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>4467</v>
+        <v>4498</v>
       </c>
       <c r="B37" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C37" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D37" s="4">
-        <v>9526.44</v>
+        <v>9632.7000000000007</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>4483</v>
+        <v>4501</v>
       </c>
       <c r="B38" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C38" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D38" s="4">
-        <v>9830.0400000000009</v>
+        <v>9922.5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>4484</v>
+        <v>4502</v>
       </c>
       <c r="B39" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C39" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D39" s="4">
-        <v>8871.1</v>
+        <v>9830.0400000000009</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>4486</v>
+        <v>4509</v>
       </c>
       <c r="B40" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C40" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D40" s="4">
-        <v>9985.5</v>
+        <v>9830.0400000000009</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>4488</v>
+        <v>4510</v>
       </c>
       <c r="B41" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C41" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D41" s="4">
-        <v>9286.5499999999993</v>
+        <v>9072.35</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>4491</v>
+        <v>4512</v>
       </c>
       <c r="B42" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C42" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D42" s="4">
-        <v>9286.5499999999993</v>
+        <v>9268.07</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>4494</v>
+        <v>4532</v>
       </c>
       <c r="B43" s="3">
-        <v>45953</v>
+        <v>45974</v>
       </c>
       <c r="C43" s="2">
-        <v>0.66034000000000004</v>
+        <v>0.65493000000000001</v>
       </c>
       <c r="D43" s="4">
-        <v>9286.5499999999993</v>
+        <v>9601.5499999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>4535</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.65493000000000001</v>
+      </c>
+      <c r="D44" s="4">
+        <v>5229.34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>4556</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.65493000000000001</v>
+      </c>
+      <c r="D45" s="4">
+        <v>7739.55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>4557</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.65493000000000001</v>
+      </c>
+      <c r="D46" s="4">
+        <v>7739.55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>4580</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.65493000000000001</v>
+      </c>
+      <c r="D47" s="4">
+        <v>7739.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>4241</v>
+      </c>
+      <c r="B48" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D48" s="4">
+        <v>29172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>4342</v>
+      </c>
+      <c r="B49" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D49" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>4380</v>
+      </c>
+      <c r="B50" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D50" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>4382</v>
+      </c>
+      <c r="B51" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D51" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>4385</v>
+      </c>
+      <c r="B52" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D52" s="4">
+        <v>14560.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>4387</v>
+      </c>
+      <c r="B53" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D53" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>4416</v>
+      </c>
+      <c r="B54" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D54" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>4419</v>
+      </c>
+      <c r="B55" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D55" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>4436</v>
+      </c>
+      <c r="B56" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D56" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>4439</v>
+      </c>
+      <c r="B57" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D57" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>4454</v>
+      </c>
+      <c r="B58" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D58" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>4458</v>
+      </c>
+      <c r="B59" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D59" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>4473</v>
+      </c>
+      <c r="B60" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D60" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>4476</v>
+      </c>
+      <c r="B61" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D61" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>4477</v>
+      </c>
+      <c r="B62" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D62" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>4517</v>
+      </c>
+      <c r="B63" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D63" s="4">
+        <v>14244.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>4524</v>
+      </c>
+      <c r="B64" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D64" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>4546</v>
+      </c>
+      <c r="B65" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D65" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>4575</v>
+      </c>
+      <c r="B66" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D66" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>4586</v>
+      </c>
+      <c r="B67" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D67" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>4597</v>
+      </c>
+      <c r="B68" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D68" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>4599</v>
+      </c>
+      <c r="B69" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D69" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>4603</v>
+      </c>
+      <c r="B70" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D70" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>4651</v>
+      </c>
+      <c r="B71" s="3">
+        <v>45981</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.65054000000000001</v>
+      </c>
+      <c r="D71" s="4">
+        <v>14586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>